<commit_message>
Cambios en app.py para prueba y producción
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,6 +981,54 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>II</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MOLINO</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CABEZAS CONTRERAS KELVIN BRATH</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>MAYRA PILAMUNGA</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>rgrtgr</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se hace cambios para añadir la base de datos
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,6 +1029,66 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>II</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>jfsdjfldsk</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>BUSTAMANTE MERCHAN RONALD ALEJANDRO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>PABLO ENRIQUEZ</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>vdjxlkvjcxlk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se añade el metodo /get-areas
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-08-28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>xxxxxxxx</t>
+          <t>II</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>xxxxxxxxxxxx</t>
+          <t>MOLINO</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>xxxxxxxx</t>
+          <t>BARRE SARANGO JONATHAN VINICIO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -573,34 +573,34 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>No aplica</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
       <c r="P2" t="inlineStr">
         <is>
           <t>Cumple</t>
@@ -608,34 +608,34 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>xxxxx</t>
+          <t>VERA BURNEO LUIS RAMIRO</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>xxxxxx</t>
+          <t>FJSLKJDASLKJDA</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-16</t>
+          <t>2024-08-29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dsada</t>
+          <t>II</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dsadas</t>
+          <t>dsalkdjlsakd</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dsada</t>
+          <t>BONE ERAZO SANDRA ELIZABETH</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -645,17 +645,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -665,12 +665,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -700,34 +700,34 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>adasdas</t>
+          <t>GAVILANEZ QUISPE EDWIN ORLANDO</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>dsadsad</t>
+          <t>dsadddddddddddddddddddddddd</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-08-29</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>II</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>XXXXXXXXX</t>
+          <t>dsadsada</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>BALSECA ALEGRIA MARCELA DEL PILAR</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -737,12 +737,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -762,12 +762,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -777,12 +777,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -792,19 +792,19 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Marta Sánchez</t>
+          <t>VILLA BALCAZAR LENIN ARMANDO</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>DADASDSADSASDA</t>
+          <t>dasdsad</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-08-29</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -814,12 +814,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MOLINO</t>
+          <t>dsadsada</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PEREZ HERRERA DENNIS ANDRES</t>
+          <t>BOLANOS ORTIZ EDGAR ARTURO</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -827,87 +827,47 @@
           <t>Cumple</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>EDWIN GAVILANEZ</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr"/>
+          <t>RIOS ALCIVAR ERICK RICARDO</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>sdgsgfd</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-22</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>III</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MOLINO</t>
+          <t>BODEGA 1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CABEZAS CONTRERAS KELVIN BRATH</t>
+          <t>BALSECA ALEGRIA MARCELA DEL PILAR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -917,12 +877,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -937,22 +897,22 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>No cumple</t>
+          <t>Cumple</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Cumple</t>
+          <t>No cumple</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -972,34 +932,34 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>DAVID NACIMBA</t>
+          <t>QUEZADA ALBAN DARWIN EDUARDO</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>dasihfhoidhfihfls</t>
+          <t>sadadadad</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-23</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>I</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MOLINO</t>
+          <t>BODEGA 5 - PASTIFICIO</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CABEZAS CONTRERAS KELVIN BRATH</t>
+          <t>CORREA ESPINOSA DIANA JESSELA</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1007,85 +967,69 @@
           <t>No cumple</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>No cumple</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Cumple</t>
+        </is>
+      </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>MAYRA PILAMUNGA</t>
+          <t>QUISPE TOAPANTA SEGUNDO ARMANDO</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>rgrtgr</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-23</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>II</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>jfsdjfldsk</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>BUSTAMANTE MERCHAN RONALD ALEJANDRO</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>No cumple</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Cumple</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>PABLO ENRIQUEZ</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>vdjxlkvjcxlk</t>
+          <t>tttttttttttttttttt</t>
         </is>
       </c>
     </row>

</xml_diff>